<commit_message>
fix: fixed dependencies, impacts, and indicators being one string in a list instead of multiple strings in a list
</commit_message>
<xml_diff>
--- a/data/climate_actions/ipcc_mitigation_options.xlsx
+++ b/data/climate_actions/ipcc_mitigation_options.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirco\Projects\CAP\data\climate_actions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC10E407-0834-4B1A-8987-B5D1792AA93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEDB067-4E05-40C2-B544-D68DC874548A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={55E9A035-244A-4003-8C1D-80C175981CA3}</author>
-    <author>tc={9D5EEA5E-CA47-4003-91AF-82CBBFC75B37}</author>
   </authors>
   <commentList>
     <comment ref="L1" authorId="0" shapeId="0" xr:uid="{55E9A035-244A-4003-8C1D-80C175981CA3}">
@@ -52,14 +51,6 @@
 </t>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{9D5EEA5E-CA47-4003-91AF-82CBBFC75B37}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Needs to be an array of strings [””,””,””]</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -1582,723 +1573,6 @@
     <t>{"stationary_energy": null, "transportation": null, "waste": "40-59", "ippu": null, "afolu": null}</t>
   </si>
   <si>
-    <t>["Policy support for land-use planning, public acceptance, and reallocation of transport budgets towards sustainable modes."]</t>
-  </si>
-  <si>
-    <t>["Investment in safe walking and cycling infrastructure, public awareness campaigns, and supportive urban planning policies."]</t>
-  </si>
-  <si>
-    <t>["Investments in modern and efficient transit systems, policies to disincentivize private car use, and public awareness campaigns to encourage public transit adoption."]</t>
-  </si>
-  <si>
-    <t>["Technological innovation, adoption of circular economy practices, and behavioral shifts towards minimalism and efficiency."]</t>
-  </si>
-  <si>
-    <t>["Development of efficient shared mobility platforms, supportive urban policies, and technological advancements in ride-sharing systems."]</t>
-  </si>
-  <si>
-    <t>["Widespread access to high-speed internet, supportive organizational policies, and employee willingness to adopt teleworking."]</t>
-  </si>
-  <si>
-    <t>["Widespread adoption of ICT and IoT technologies, supportive urban planning, and investments in shared and digitalized mobility systems."]</t>
-  </si>
-  <si>
-    <t>["Access to advanced logistics tools and software, collaboration between supply chain stakeholders, and integration of eco-driving training"]</t>
-  </si>
-  <si>
-    <t>["Expansion of e-commerce platforms, investments in last-mile delivery logistics, and consumer trust in online shopping."]</t>
-  </si>
-  <si>
-    <t>["Development and deployment of autonomous vehicle technologies, supportive regulatory frameworks, and public acceptance of automated systems."]</t>
-  </si>
-  <si>
-    <t>["Development of low-cost and sustainable production technologies, supportive policy measures (e.g., fuel standards, blending mandates), and investment in distribution and storage infrastructure."]</t>
-  </si>
-  <si>
-    <t>["Dependence on advancements in battery technologies, development of charging infrastructure, policies for subsidies and incentives, and integration with renewable energy sources for electricity generation."]</t>
-  </si>
-  <si>
-    <t>["Hydrogen production infrastructure, availability of low-carbon hydrogen, cost reductions in fuel cell systems, and durable policies to support adoption."]</t>
-  </si>
-  <si>
-    <t>["Availability and development of advanced lightweight materials, efficient recycling processes, and industry-scale implementation."]</t>
-  </si>
-  <si>
-    <t>["Development and deployment of advanced vehicle technologies, regulatory frameworks, and consumer acceptance."]</t>
-  </si>
-  <si>
-    <t>["Driver education, effective training programs, policy support, and incentive mechanisms to encourage adoption of eco-driving practices."]</t>
-  </si>
-  <si>
-    <t>["Development and adoption of advanced aircraft technology, global air traffic management optimization, and industry investments in research and development."]</t>
-  </si>
-  <si>
-    <t>["Availability of low-carbon energy, advancements in fuel production technologies, cost reductions, policy support, and infrastructure for production and distribution."]</t>
-  </si>
-  <si>
-    <t>["Requires significant investments in HSR infrastructure, policy support to limit competing air travel options, and integration of rail networks with existing transportation systems."]</t>
-  </si>
-  <si>
-    <t>["Availability of low-carbon fuels and energy, infrastructure investments, retrofitting capabilities for existing ships, policy and regulatory support, and advances in fuel storage and safety technologies."]</t>
-  </si>
-  <si>
-    <t>["Availability of low-carbon electricity, advancements in battery technology, infrastructure for charging and maintenance, and supportive regulatory frameworks for the maritime industry."]</t>
-  </si>
-  <si>
-    <t>["Availability of low-carbon fuels, advancements in propulsion and hull design technologies, investments in port infrastructure, and regulatory support for energy efficiency and emissions reductions."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced technologies, supportive regulatory frameworks, investment in research and development, and alignment with global standards for emissions reduction and energy efficiency."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced fuel delivery systems, supportive policy frameworks, investment in R&amp;D for alternative reductants, and industry-wide adoption of optimized process controls and technologies."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced furnace designs, supportive policies and incentives, skilled workforce for installation and maintenance, and industry-wide adoption of energy-efficient technologies."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced heat recovery and pump technologies, skilled workforce for installation and maintenance, and policy support for adoption of waste heat recovery systems."]</t>
-  </si>
-  <si>
-    <t>["Development and deployment of advanced process integration technologies, skilled workforce training, and supportive policies to incentivize adoption."]</t>
-  </si>
-  <si>
-    <t>["Development of advanced comminution and ore sorting technologies, availability of renewable energy sources for power generation, and policy support to incentivize adoption."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced drying/dewatering technologies, skilled workforce for implementation, and supportive policies or incentives to offset initial costs."]</t>
-  </si>
-  <si>
-    <t>["Availability of recycling infrastructure, advanced technologies for material separation and recovery, and supportive policies for incentivizing recycling practices."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced technologies like sensors and machine learning systems, adequate digital infrastructure, and supportive policies for energy efficiency adoption."]</t>
-  </si>
-  <si>
-    <t>["Availability of renewable fuel infrastructure, technology development for alternative fuel production, and supportive policies."]</t>
-  </si>
-  <si>
-    <t>["Availability of low-carbon electricity, development of suitable anode materials, and infrastructure for large-scale electrification in steel production."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced heat recovery technologies, skilled workforce for installation and operation, and supportive policies and funding incentives."]</t>
-  </si>
-  <si>
-    <t>["Development of advanced process technologies, regulatory support for adoption, workforce training, and sufficient financial incentives or subsidies to offset high initial costs."]</t>
-  </si>
-  <si>
-    <t>["Access to biomass resources, skilled workforce for CHP system operation, and supportive policies to incentivize adoption of CHP systems."]</t>
-  </si>
-  <si>
-    <t>["Requires advancements in CCS and CCU technologies, availability of low-GHG electricity, and supportive policies to incentivize industrial decarbonization."]</t>
-  </si>
-  <si>
-    <t>["Availability of clean energy for hydrogen production, development of CCU technologies, and policies to support adoption."]</t>
-  </si>
-  <si>
-    <t>["Requires the development of CO2 transport and storage infrastructure, supportive policy frameworks, sufficient clean energy for capture processes, and incentives for adoption."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced materials, supportive policies for circular economy, stakeholder collaboration across supply chains, and investment in R&amp;D for lightweight materials and high-efficiency design methods."]</t>
-  </si>
-  <si>
-    <t>["Availability of advanced manufacturing technologies, workforce training, supportive regulations, and access to materials for near-net shape casting."]</t>
-  </si>
-  <si>
-    <t>["Collaboration across supply chains, advances in recycling and remanufacturing technologies, and supportive policy frameworks to incentivize adoption."]</t>
-  </si>
-  <si>
-    <t>["Effective coordination between industries, governments, and communities; supportive policies and regulations; development of recycling infrastructure; and data sharing platforms for material and energy flows."]</t>
-  </si>
-  <si>
-    <t>["Development and availability of alternative feedstocks, regulatory support for material substitution, and investment in research and development for innovative concrete applications."]</t>
-  </si>
-  <si>
-    <t>["Availability of infrastructure for waste collection and recycling, public awareness campaigns, and supportive policy frameworks."]</t>
-  </si>
-  <si>
-    <t>["Requires clear guidelines, consumer education campaigns, and industry compliance with precise dosing recommendations."]</t>
-  </si>
-  <si>
-    <t>["Development of platforms and systems to facilitate product sharing, stakeholder collaboration, and supportive policies to incentivize shared usage models."]</t>
-  </si>
-  <si>
-    <t>["Requires collaboration across material supply chains, advancements in product design, and supportive policy frameworks to incentivize circular economy practices."]</t>
-  </si>
-  <si>
-    <t>["Development of advanced maintenance techniques, effective policies to promote longer building lifespans, and education for construction professionals on durable practices."]</t>
-  </si>
-  <si>
-    <t>["Public awareness campaigns, supportive policies, and integration of sustainability into business and governmental frameworks."]</t>
-  </si>
-  <si>
-    <t>["Implementation of policies and programs promoting sustainable consumption, availability of alternatives to high-emission activities, and societal support for behavioral and lifestyle changes."]</t>
-  </si>
-  <si>
-    <t>["Requires improved governance, clear land tenure policies, funding for protected areas, and community participation in forest conservation efforts."]</t>
-  </si>
-  <si>
-    <t>["Requires funding for land restoration, access to suitable species for planting, local community engagement, and monitoring systems for ecosystem integrity and carbon sequestration."]</t>
-  </si>
-  <si>
-    <t>["Requires expertise in sustainable forestry, investment in nurseries with adapted species, supportive policies, and incentives to overcome economic barriers and ensure accessibility for local stakeholders."]</t>
-  </si>
-  <si>
-    <t>["Effective governance frameworks, access to research and technology for fire management, community engagement, and alignment with regional legal and policy frameworks."]</t>
-  </si>
-  <si>
-    <t>["Strong policy frameworks, financial incentives for conservation, and collaboration between governments, local communities, and landowners to implement sustainable practices."]</t>
-  </si>
-  <si>
-    <t>["Requires strong governance, financial support, international cooperation, and policies to control land conversion drivers such as agriculture, mining, and urban development."]</t>
-  </si>
-  <si>
-    <t>["Availability of funding, collaboration among local and national stakeholders, scientific research on optimal restoration practices, and policies to incentivize restoration efforts."]</t>
-  </si>
-  <si>
-    <t>["Effective integration of coastal climate mitigation policies, marine spatial planning, and economic incentives to prioritize wetland conservation."]</t>
-  </si>
-  <si>
-    <t>["Requires long-term commitments, supportive policies, funding, monitoring frameworks, and technical capacity to address drivers of degradation and ensure restoration success."]</t>
-  </si>
-  <si>
-    <t>["Success depends on the availability of resources for monitoring and verification, regional adaptation of practices, and addressing barriers such as soil saturation and permanence issues."]</t>
-  </si>
-  <si>
-    <t>["Availability of sustainably sourced biomass, standardization of production methods, monitoring systems, and incentives for scaling up biochar production and application."]</t>
-  </si>
-  <si>
-    <t>["Requires access to appropriate germplasm, supportive policies, extension systems, credit access, and reforms in land tenure systems. Adoption depends on aligning agroforestry practices to biophysical and socio-economic contexts."]</t>
-  </si>
-  <si>
-    <t>["Development and regulatory approval of feed additives, vaccines, and inhibitors; regional adaptation of mitigation strategies; and overcoming barriers like costs, infrastructure, and public acceptance."]</t>
-  </si>
-  <si>
-    <t>["Adequate irrigation infrastructure, training for farmers on advanced techniques, access to slow-release fertilisers and biochar, and coordinated water management practices among neighboring farmers and regions."]</t>
-  </si>
-  <si>
-    <t>["Availability of training and technical support for farmers, development of regional nutrient management roadmaps, and access to affordable fertilizers and inhibitors."]</t>
-  </si>
-  <si>
-    <t>["Development of cost-effective anaerobic digestion systems, supportive policies for nitrification inhibitors, region-specific training programs, and accessible financing for farmers."]</t>
-  </si>
-  <si>
-    <t>["Requires sustainable land management, advanced bioenergy technology development, infrastructure for carbon capture and storage, and global governance for trade and supply chains."]</t>
-  </si>
-  <si>
-    <t>["Implementation of integrated food-system policies, financial incentives for sustainable agriculture, awareness campaigns, and the development of local food systems to support dietary transitions."]</t>
-  </si>
-  <si>
-    <t>["Adequate infrastructure for food storage and transportation, policy frameworks for waste reduction, financial incentives, and widespread consumer education to change behaviors."]</t>
-  </si>
-  <si>
-    <t>["Requires sustainable forest management practices, advanced wood processing technologies, market demand for wood substitutes, and global cooperation to prevent resource exploitation."]</t>
-  </si>
-  <si>
-    <t>["Requires integrated spatial planning, infrastructure development, zoning regulations, and public transport investment."]</t>
-  </si>
-  <si>
-    <t>["Requires effective urban planning, policy support for mixed land use, investment in public transit infrastructure, and cooperation across municipal agencies."]</t>
-  </si>
-  <si>
-    <t>["High institutional capacity for cross-sector collaboration, advanced GIS tools for spatial planning, and stakeholder engagement for co-design processes."]</t>
-  </si>
-  <si>
-    <t>["Requires grid upgrades, supportive policies, stakeholder cooperation, financial incentives, and public awareness campaigns, access to renewable energy and advanced storage technologies is critical."]</t>
-  </si>
-  <si>
-    <t>["Sustainable forestry management, international carbon accounting standards, development of mass timber technologies, robust forest and urban land governance policies, and incentivized afforestation practices."]</t>
-  </si>
-  <si>
-    <t>["Availability of land for planting, community participation, funding for maintenance, and policies supporting urban greening initiatives"]</t>
-  </si>
-  <si>
-    <t>["Requires local government coordination, community engagement, urban planning integration, and adequate funding for infrastructure development and maintenance."]</t>
-  </si>
-  <si>
-    <t>["Requires integrated urban planning, investment in active transport infrastructure, collaboration between urban and transportation planners, and community engagement."]</t>
-  </si>
-  <si>
-    <t>["Requires institutional capacity, governance, cross-sectoral coordination, and public awareness campaigns, needs infrastructure for decentralized waste treatment and policies to promote circular economy practices."]</t>
-  </si>
-  <si>
-    <t>["Reduction in per capita car use, increase in public transport ridership, improved walkability index."]</t>
-  </si>
-  <si>
-    <t>["Increase in kilometers of bicycle and walking networks, rise in active transport modal share, reduction in car usage for short trips."]</t>
-  </si>
-  <si>
-    <t>["Increase in public transit ridership, reduction in private vehicle kilometers traveled, and emissions reduction per passenger kilometer."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material intensity per unit output, decrease in freight transport emissions, and increased adoption of circular economy practices."]</t>
-  </si>
-  <si>
-    <t>["Increase in shared mobility trips, reduction in private vehicle kilometers traveled, and decreased transport-related emissions."]</t>
-  </si>
-  <si>
-    <t>["Reduction in commuter trips, increase in teleworking adoption rates, and decreased transport-related emissions."]</t>
-  </si>
-  <si>
-    <t>["Increase in shared and public transport use, reduction in private vehicle kilometers traveled, and decreased transport-related emissions."]</t>
-  </si>
-  <si>
-    <t>["Reduced freight distances, increased vehicle carrying capacity, improved fuel efficiency, and reduced operating costs"]</t>
-  </si>
-  <si>
-    <t>["Reduction in vehicle kilometers traveled (VMT) for shopping, increase in online shopping adoption rates, and emissions reductions in freight logistics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in congestion, improved fuel efficiency, decreased transport-related emissions per vehicle kilometer, and increased accessibility for marginalized groups."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions from fuel lifecycle, percentage of vehicle fleet using alternative fuels, and infrastructure deployment metrics."]</t>
-  </si>
-  <si>
-    <t>["Percentage of electric vehicles in the vehicle fleet, reduction in GHG emissions per kilometer traveled, and availability of charging infrastructure."]</t>
-  </si>
-  <si>
-    <t>["Share of fuel cell vehicles in the vehicle fleet, reduction in GHG emissions per kilometer, deployment of hydrogen refueling stations, cost parity with diesel vehicles."]</t>
-  </si>
-  <si>
-    <t>["Reduction in vehicle mass, improvement in fuel efficiency (km/l), lifecycle GHG emissions avoided, and share of lightweighted vehicles in the fleet."]</t>
-  </si>
-  <si>
-    <t>["Improvements in fuel economy (km/l), reduction in GHG emissions per km, share of energy-efficient vehicles in fleets, and fuel cost savings."]</t>
-  </si>
-  <si>
-    <t>["Percentage reduction in fuel consumption, GHG emissions per vehicle, number of drivers trained in eco-driving, and adherence to eco-driving practices among trained drivers."]</t>
-  </si>
-  <si>
-    <t>["Percentage reduction in fuel consumption per flight, improvement in navigation efficiency, and adoption rate of advanced aircraft designs."]</t>
-  </si>
-  <si>
-    <t>["Adoption rates of SAFs, lifecycle emissions reductions, and advancements in fuel production technologies."]</t>
-  </si>
-  <si>
-    <t>["Reduction in domestic and regional air travel demand, increase in HSR ridership, and measurable reductions in transportation sector GHG emissions."]</t>
-  </si>
-  <si>
-    <t>["Adoption rate of alternative fuels, emissions reductions achieved (tank-to-wake and well-to-wake), and advancements in bunkering and storage infrastructure."]</t>
-  </si>
-  <si>
-    <t>["Reduction in lifecycle emissions of vessels, number of electric and hybrid-electric ships in operation, and improvements in port infrastructure to support electric propulsion systems."]</t>
-  </si>
-  <si>
-    <t>["Reduction in shipping emissions, adoption rate of energy-efficient technologies and operational measures, number of retrofitted vessels, and efficiency improvements in port operations."]</t>
-  </si>
-  <si>
-    <t>["Reduction in industrial GHG emissions, adoption rates of heat and energy recovery technologies, energy intensity improvements in key industries, and recycling rates."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions from heating in steel production, energy intensity improvements, increased adoption rates of pulverized coal injection and alternative fuels, and reduced production of hazardous wastes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy intensity, GHG emissions, and hazardous waste production; increased adoption of advanced furnaces and process controls."]</t>
-  </si>
-  <si>
-    <t>["Increase in waste heat recovery rate, reduction in energy intensity, and percentage of heat reused through high-efficiency systems."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy consumption per unit of steel, increase in process coupling efficiency, and reduction in GHG emissions per ton of steel produced."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy consumption per ton of ore processed, improvement in ore recovery ratio, and reduction in GHG emissions from mining operations."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy consumption per unit of output, percentage improvement in drying efficiency, and reduction in GHG emissions from manufacturing processes."]</t>
-  </si>
-  <si>
-    <t>["Recycling rates by material type, reduction in energy consumption for material production, and decrease in landfill waste volumes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy use, cost savings per production cycle, and percentage improvement in process efficiency."]</t>
-  </si>
-  <si>
-    <t>["Reduction in CO2 emissions, increased adoption rate of renewable fuels, and reduction in the carbon intensity of industrial processes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in emissions per ton of steel produced, increase in the share of electrified processes, and energy savings in production stages."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy consumption per ton of product, increase in waste energy recovery rates, and decrease in GHG emissions intensity in industrial processes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy use per unit of production, lower emissions per ton of material produced, increased adoption rate of advanced technologies, and improved process efficiency metrics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in energy intensity per ton of paper, decrease in direct and indirect CO2 emissions, and increase in on-site electricity production through CHP systems."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions from industrial processes, increase in the use of low-carbon feedstocks, and the number of CCS/CCU projects implemented."]</t>
-  </si>
-  <si>
-    <t>["Quantity of CO2 captured and reused, reduction in emissions per ton of product, and market penetration of CCU-derived products."]</t>
-  </si>
-  <si>
-    <t>["Amount of CO2 captured and stored annually, percentage reduction in industrial emissions, and operational capacity of CCS projects globally."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material usage per product, increase in product lifespan, percentage of materials recovered and reused, and reduction in GHG emissions from production processes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material waste, increase in production yield, and reduction in GHG emissions per unit of material produced."]</t>
-  </si>
-  <si>
-    <t>["Percentage of materials recovered and reused, reduction in production waste, and decrease in GHG emissions per unit of product lifecycle."]</t>
-  </si>
-  <si>
-    <t>["Reduction in virgin material use, GHG emissions avoided through CE practices, increase in recycling rates, number of industrial symbiosis networks implemented, and resource recovery metrics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in clinker-to-cement ratio, lower CO2 emissions per tonne of cement, and increased adoption of alternative materials in cement production."]</t>
-  </si>
-  <si>
-    <t>["Reduction in food waste percentage, increased recycling rates, and reduced greenhouse gas emissions from waste management."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material waste, increased adherence to dosing guidelines, and measurable decreases in associated emissions."]</t>
-  </si>
-  <si>
-    <t>["Number of shared product-service systems implemented, reduction in material demand per capita, and decrease in GHG emissions from product manufacturing."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material use per product, increase in product lifespan, rate of reuse and repair, and reduction in GHG emissions from material production and waste."]</t>
-  </si>
-  <si>
-    <t>["Increase in the average lifespan of buildings and infrastructure, reduction in cement demand per capita, and overall CO2 emissions reductions in cement production."]</t>
-  </si>
-  <si>
-    <t>["Reduction in material and energy intensity per capita, decrease in waste generation rates, and improvement in recycling and reuse statistics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in demand for high-emission products and services, decreased industrial emissions linked to product use, and increased adoption of sustainable consumption practices."]</t>
-  </si>
-  <si>
-    <t>["Reduction in deforestation rates, increased forest cover, and the amount of GHG emissions avoided per year."]</t>
-  </si>
-  <si>
-    <t>["Area of land reforested or afforested, carbon sequestration rates, improvement in biodiversity indices, and ecosystem service metrics such as water regulation and soil quality."]</t>
-  </si>
-  <si>
-    <t>["Increase in forest carbon stocks, reduction in GHG emissions, improvements in biodiversity indicators, and reduction in soil erosion and water-related issues."]</t>
-  </si>
-  <si>
-    <t>["Reduction in frequency and intensity of uncontrolled wildfires, area managed with prescribed burns, reduction in GHG emissions from fires, and improvement in biodiversity and soil health metrics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in conversion rates of grasslands, increase in soil organic carbon levels, and measurable reduction in GHG emissions from targeted areas."]</t>
-  </si>
-  <si>
-    <t>["Reduction in peatland conversion rates, avoided emissions per hectare, and improvements in biodiversity and water quality metrics."]</t>
-  </si>
-  <si>
-    <t>["Area of coastal wetlands preserved, GHG emissions avoided from biomass and soil carbon loss, and improvements in biodiversity metrics and ecosystem resilience."]</t>
-  </si>
-  <si>
-    <t>["Area of wetlands restored, carbon sequestration rates, biodiversity recovery metrics, reduction in storm damage costs, and water quality improvements."]</t>
-  </si>
-  <si>
-    <t>["Increase in soil organic carbon, reduction in GHG emissions, improvement in agricultural productivity, and biodiversity enhancements."]</t>
-  </si>
-  <si>
-    <t>["Carbon sequestration rates, reduction in soil N2O emissions, crop yield improvements, and displacement of fossil fuel use through pyrolysis gases."]</t>
-  </si>
-  <si>
-    <t>["Carbon sequestration rates (above and below ground), improved soil health metrics, increase in farmer income, reduction in soil erosion, and adoption rates of agroforestry systems."]</t>
-  </si>
-  <si>
-    <t>["Reduction in CH4 emissions per animal, adoption rates of improved feeding practices, and increase in production efficiency per unit of livestock product."]</t>
-  </si>
-  <si>
-    <t>["Reduction in CH4 and N2O emissions per hectare, increased water use efficiency, yield stability during droughts, and adoption rate of improved rice cultivation techniques."]</t>
-  </si>
-  <si>
-    <t>["Reduction in N2O emissions, improvement in crop yields, increase in soil carbon sequestration, and reduction in fertilizer use per hectare."]</t>
-  </si>
-  <si>
-    <t>["Reduction in CH4 and N2O emissions from manure storage, increased adoption of anaerobic digestion systems, improved nitrogen use efficiency, and enhanced biogas production."]</t>
-  </si>
-  <si>
-    <t>["Amount of carbon removed through BECCS (in GtCO2 per year), total energy produced from bioenergy, land restored for biomass production, and GHG emissions reduction from displaced fossil fuel use."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions from food production, reduction in land use for livestock, increase in plant-based food consumption, and improvement in public health metrics related to diet-related diseases."]</t>
-  </si>
-  <si>
-    <t>["Reduction in food waste percentages at consumer and business levels, decrease in land used for agricultural production, and measurable GHG emission reductions across the food supply chain."]</t>
-  </si>
-  <si>
-    <t>["Increased use of wood products in construction, reduction in GHG emissions from material substitution, and increase in recycled wood product utilization rates."]</t>
-  </si>
-  <si>
-    <t>["Reduction in vehicle miles traveled, increase in public transport usage, percentage of urban areas with mixed-use development, and lower per capita energy use in urban areas."]</t>
-  </si>
-  <si>
-    <t>["Reduction in VMT, increase in public transit ridership, decrease in transport-related GHG emissions, and improved accessibility to jobs and housing."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions per capita, adoption rates of district heating/cooling systems, and proportion of urban population with access to green areas."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions per kWh, increase in renewable energy penetration, adoption rates of EVs and heat pumps, and improved urban air quality."]</t>
-  </si>
-  <si>
-    <t>["Reduction in embodied carbon in construction, number of mid-rise urban buildings using engineered timber, carbon sequestration capacity of urban timber infrastructure, and improvement in sustainable forestry practices."]</t>
-  </si>
-  <si>
-    <t>["Increase in urban tree cover percentage, reduction in urban heat island effect, amount of carbon sequestered, reduction in building energy use, and improvement in air quality metrics."]</t>
-  </si>
-  <si>
-    <t>["Reduction in building energy consumption, increase in urban green coverage, stormwater retention rates, increased active transportation use (cycling/walking), and improved thermal comfort."]</t>
-  </si>
-  <si>
-    <t>["Reduction in vehicle miles traveled (VMT), increase in walking and biking trips, reduction in urban GHG emissions, and improved accessibility to essential services."]</t>
-  </si>
-  <si>
-    <t>["Reduction in waste generation per capita, increase in recycling and composting rates, reduction in CH4 emissions from waste, and employment opportunities created in waste management."]</t>
-  </si>
-  <si>
-    <t>["Improved urban livability, better public health outcomes, reduced GHG emissions."]</t>
-  </si>
-  <si>
-    <t>["Improved public health, reduced urban congestion, lower transport-related GHG emissions, and enhanced quality of urban life."]</t>
-  </si>
-  <si>
-    <t>["Enhanced urban livability, reduced traffic congestion, improved public health, and significant reductions in transport-related greenhouse gas emissions."]</t>
-  </si>
-  <si>
-    <t>["Improved resource efficiency, lower environmental footprint, and potential for reduced transport emissions."]</t>
-  </si>
-  <si>
-    <t>["Enhanced urban mobility, reduced traffic congestion, lower transport emissions, and increased system efficiency."]</t>
-  </si>
-  <si>
-    <t>["Reduced traffic congestion, improved air quality, enhanced work-life balance, and lower transport emissions."]</t>
-  </si>
-  <si>
-    <t>["Enhanced urban livability, reduced congestion, improved air quality, and significant advancements in transport efficiency."]</t>
-  </si>
-  <si>
-    <t>["Reduced operating costs, improved corporate image, enhanced transport infrastructure utilisation, and potential air quality improvement"]</t>
-  </si>
-  <si>
-    <t>["Improved urban mobility, reduced shopping-related travel emissions, and enhanced convenience for consumers."]</t>
-  </si>
-  <si>
-    <t>["Enhanced road safety, reduced traffic congestion, increased accessibility for underserved populations, and optimization of transport systems for environmental and societal benefit."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, improved air quality, energy diversification, and increased resilience in transportation systems."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, improved urban air quality, decreased reliance on fossil fuels, and greater energy security."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, improved air quality, energy diversification, and advancement of clean technologies for transportation."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced fuel efficiency, improved vehicle performance, and contribution to a circular economy through advanced recycling."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced fuel efficiency, lower operating costs, and improved air quality."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced fuel efficiency, improved road safety, and lower transport costs."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced operational efficiency, and strengthened energy security in aviation."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in aviation emissions, improved energy security, and progress toward net-zero aviation operations."]</t>
-  </si>
-  <si>
-    <t>["Reduces aviation emissions, improves regional connectivity, decreases transportation-related air pollution, and enhances public transportation networks."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in maritime emissions, improved air quality, progress toward global decarbonization goals, and reduced reliance on fossil fuels in the shipping industry."]</t>
-  </si>
-  <si>
-    <t>["Significant reduction in maritime sector emissions, improved air quality in coastal and port regions, decreased reliance on fossil fuels, and promotion of innovation in clean transportation technologies."]</t>
-  </si>
-  <si>
-    <t>["Reduction in maritime emissions, improved air and water quality, increased energy security, and enhanced innovation in sustainable shipping technologies."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in industrial emissions, improved resource efficiency, enhanced energy security, and increased sustainability in manufacturing and construction sectors."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in emissions and energy use in steel manufacturing, improved air quality, enhanced energy security, and more sustainable industrial practices."]</t>
-  </si>
-  <si>
-    <t>["Significant improvements in industrial energy efficiency, reduced emissions, cost savings for manufacturers, and enhanced air quality."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in industrial energy consumption and GHG emissions, enhanced energy security, cost savings for manufacturers, and reduced environmental waste."]</t>
-  </si>
-  <si>
-    <t>["Improved energy efficiency, reduced emissions, cost savings for manufacturers, and enhanced competitiveness of the steel industry in global markets."]</t>
-  </si>
-  <si>
-    <t>["Improved energy efficiency in mining, reduced operational costs, decreased environmental footprint of mining activities, and enhanced resource utilization."]</t>
-  </si>
-  <si>
-    <t>["Increased energy efficiency, reduced operational costs, lower emissions, and enhanced sustainability in industrial processes."]</t>
-  </si>
-  <si>
-    <t>["Reduces reliance on virgin material extraction, lowers industrial energy demand, mitigates GHG emissions, and supports sustainable production practices."]</t>
-  </si>
-  <si>
-    <t>["Enhanced energy efficiency, reduced operational costs, improved industrial competitiveness, and support for decarbonization goals."]</t>
-  </si>
-  <si>
-    <t>["Reduced dependence on fossil fuels, improved energy security, and mitigation of air pollution, contributing to global emission reduction targets."]</t>
-  </si>
-  <si>
-    <t>["Reduced reliance on fossil fuels, improved air quality, and enhanced global competitiveness of steel manufacturers."]</t>
-  </si>
-  <si>
-    <t>["Enhances energy efficiency, reduces emissions, lowers operational costs, and improves competitiveness of the industrial sector in global markets."]</t>
-  </si>
-  <si>
-    <t>["Enhanced energy efficiency, significant emissions reductions, cost savings for industries, increased competitiveness in global markets, and improved environmental sustainability."]</t>
-  </si>
-  <si>
-    <t>["Improved energy efficiency, reduced emissions, enhanced competitiveness of the pulp and paper industry, and long-term cost savings for manufacturers."]</t>
-  </si>
-  <si>
-    <t>["Enhanced industrial sustainability, reduced dependence on fossil fuels, advancement of circular economy principles, and mitigation of climate change impacts."]</t>
-  </si>
-  <si>
-    <t>["Reduction in GHG emissions, enhanced energy security, and development of sustainable industries."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in GHG emissions, mitigation of climate change effects, and increased energy security through sustainable industrial practices."]</t>
-  </si>
-  <si>
-    <t>["Reduced environmental footprint, lower production costs, improved resource efficiency, and enhanced sustainability of industrial processes."]</t>
-  </si>
-  <si>
-    <t>["Significant reduction in material and energy use, enhanced production efficiency, reduced emissions, and improved sustainability across industrial supply chains."]</t>
-  </si>
-  <si>
-    <t>["Reduction in raw material demand, improved environmental sustainability, decreased emissions, and enhanced industrial efficiency."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in resource extraction, energy use, and emissions; enhanced regional development through eco-industrial parks; and broader adoption of sustainable practices across industries and urban areas."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced resource efficiency, lower energy consumption in cement production, and improved environmental quality in cement manufacturing regions."]</t>
-  </si>
-  <si>
-    <t>["Reduced environmental burden, enhanced resource efficiency, improved urban livability, and cost savings in waste management systems."]</t>
-  </si>
-  <si>
-    <t>["Reduced industrial emissions, lower resource consumption, cost savings for consumers and industries, and improved efficiency across the supply chain."]</t>
-  </si>
-  <si>
-    <t>["Reduction in resource use and emissions, cost savings for consumers, increased accessibility to products, and fostering a circular economy through more efficient use of materials."]</t>
-  </si>
-  <si>
-    <t>["Significant emissions reductions, resource conservation, cost savings for consumers, and strengthened circular economy practices."]</t>
-  </si>
-  <si>
-    <t>["Reduction in demand for new concrete and cement production, reduced emissions, enhanced resource efficiency, and increased affordability and sustainability of infrastructure."]</t>
-  </si>
-  <si>
-    <t>["Enhances societal well-being by reducing overconsumption, lowering environmental impacts, and fostering long-term sustainability in resource use and industrial processes."]</t>
-  </si>
-  <si>
-    <t>["Reduction in global GHG emissions, improved resource efficiency, enhanced sustainability in consumption patterns, and reduced strain on environmental resources."]</t>
-  </si>
-  <si>
-    <t>["Preserves biodiversity, enhances ecosystem services, improves air and water quality, and contributes to climate stabilization and sustainable development."]</t>
-  </si>
-  <si>
-    <t>["Increased carbon sequestration, improved biodiversity, enhanced ecosystem resilience, better water regulation, soil stabilization, and support for local communities through sustainable resource use."]</t>
-  </si>
-  <si>
-    <t>["Improved forest health and resilience, enhanced carbon sequestration, biodiversity conservation, and increased ecosystem services like water and soil regulation."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, improved biodiversity conservation, prevention of soil erosion, enhanced land productivity, and reduced risks to life and property from uncontrolled wildfires."]</t>
-  </si>
-  <si>
-    <t>["Preserves ecosystem services, enhances biodiversity, supports climate resilience, and provides sustainable livelihoods for communities dependent on grasslands."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, enhanced biodiversity, improved water regulation, and decreased fire-related health hazards."]</t>
-  </si>
-  <si>
-    <t>["Significant reductions in CO2 emissions, improved biodiversity, enhanced water regulation, reduced flooding risks, and increased resilience to climate change."]</t>
-  </si>
-  <si>
-    <t>["Increased carbon sequestration, enhanced resilience to climate impacts, improved biodiversity, better water quality, and greater protection against flooding and storm surges."]</t>
-  </si>
-  <si>
-    <t>["Enhanced ecosystem resilience, improved carbon sequestration, protection against sea-level rise and storms, increased biodiversity, and strengthened coastal livelihoods and food security."]</t>
-  </si>
-  <si>
-    <t>["Enhanced soil health, improved water retention, increased crop yields, greater biodiversity, reduced erosion, and resilience to climate change in agricultural and grassland ecosystems."]</t>
-  </si>
-  <si>
-    <t>["Improved agricultural productivity, enhanced soil resilience to climate change, reduced pollution, and long-term carbon storage in soils, contributing to global climate goals."]</t>
-  </si>
-  <si>
-    <t>["Enhanced land productivity, improved livelihoods, increased carbon storage, better water quality, and resilience to climate change."]</t>
-  </si>
-  <si>
-    <t>["Reduction in global agricultural methane emissions, improved livestock productivity, and enhanced food security, particularly in regions with high agricultural dependence."]</t>
-  </si>
-  <si>
-    <t>["Reduced greenhouse gas emissions, improved water use efficiency, enhanced drought resilience, increased farm income, and more sustainable agricultural practices contributing to food security."]</t>
-  </si>
-  <si>
-    <t>["Contributes to climate mitigation, improves food and nutrition security, enhances environmental sustainability, and supports long-term agricultural productivity."]</t>
-  </si>
-  <si>
-    <t>["Reduces greenhouse gas emissions, improves local water and air quality, enhances soil health, supports food security, and provides renewable energy through biogas production."]</t>
-  </si>
-  <si>
-    <t>["Enhanced energy security, reduced GHG emissions, restored degraded lands, improved air and water quality, and biodiversity conservation."]</t>
-  </si>
-  <si>
-    <t>["Improved public health outcomes, reduced environmental pressures (e.g., deforestation, biodiversity loss), and strengthened food security through sustainable practices."]</t>
-  </si>
-  <si>
-    <t>["Enhances food security, reduces environmental stress on water and land resources, supports poverty alleviation, and contributes to achieving SDG 12 for sustainable consumption and production patterns."]</t>
-  </si>
-  <si>
-    <t>["Reduces emissions from traditional material production, enhances carbon sequestration, supports sustainable forest industries, and provides economic opportunities in rural and forested areas."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions, improved public health, better urban livability, reduced resource consumption, and preservation of land for agriculture and forestry."]</t>
-  </si>
-  <si>
-    <t>["Reduces GHG emissions, improves air quality, enhances urban livability, and fosters more sustainable urban growth patterns."]</t>
-  </si>
-  <si>
-    <t>["Enhanced livability, improved public health, reduced energy use, increased resilience to climate impacts, and promotion of green economic growth."]</t>
-  </si>
-  <si>
-    <t>["Enhances energy security, reduces urban air pollution, improves public health, and supports sustainable urban development through renewable energy and electrification."]</t>
-  </si>
-  <si>
-    <t>["Reduced GHG emissions from construction, enhanced carbon storage in urban environments, sustainable urbanization, improved resource efficiency, and reduced pressure on natural ecosystems."]</t>
-  </si>
-  <si>
-    <t>["Enhanced urban livability, improved public health, reduced energy consumption, increased biodiversity, and greater resilience to climate change impacts."]</t>
-  </si>
-  <si>
-    <t>["Enhanced urban livability, reduced urban heat island effects, improved public health, better stormwater management, and increased biodiversity in urban areas."]</t>
-  </si>
-  <si>
-    <t>["Reduces urban energy use, improves public health, enhances urban livability, and fosters community engagement through better connectivity and accessibility."]</t>
-  </si>
-  <si>
-    <t>["Improved urban livability, reduction in landfill emissions, enhanced resource efficiency, and economic growth through job creation in the waste management sector."]</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -2312,17 +1586,741 @@
   </si>
   <si>
     <t>BehavioralChangeTargeted</t>
+  </si>
+  <si>
+    <t>["Policy support for land-use planning", "public acceptance", "reallocation of transport budgets towards sustainable modes"]</t>
+  </si>
+  <si>
+    <t>["Investment in safe walking and cycling infrastructure", "public awareness campaigns", "supportive urban planning policies"]</t>
+  </si>
+  <si>
+    <t>["Investments in modern and efficient transit systems", "policies to disincentivize private car use", "public awareness campaigns to encourage public transit adoption"]</t>
+  </si>
+  <si>
+    <t>["Technological innovation", "adoption of circular economy practices", "behavioral shifts towards minimalism and efficiency"]</t>
+  </si>
+  <si>
+    <t>["Development of efficient shared mobility platforms", "supportive urban policies", "technological advancements in ride-sharing systems"]</t>
+  </si>
+  <si>
+    <t>["Widespread access to high-speed internet", "supportive organizational policies", "employee willingness to adopt teleworking"]</t>
+  </si>
+  <si>
+    <t>["Widespread adoption of ICT and IoT technologies", "supportive urban planning", "investments in shared and digitalized mobility systems"]</t>
+  </si>
+  <si>
+    <t>["Access to advanced logistics tools and software", "collaboration between supply chain stakeholders", "integration of eco-driving training"]</t>
+  </si>
+  <si>
+    <t>["Expansion of e-commerce platforms", "investments in last-mile delivery logistics", "consumer trust in online shopping"]</t>
+  </si>
+  <si>
+    <t>["Development and deployment of autonomous vehicle technologies", "supportive regulatory frameworks", "public acceptance of automated systems"]</t>
+  </si>
+  <si>
+    <t>["Development of low-cost and sustainable production technologies", "supportive policy measures (e.g., fuel standards, blending mandates)", "investment in distribution and storage infrastructure"]</t>
+  </si>
+  <si>
+    <t>["Dependence on advancements in battery technologies", "development of charging infrastructure", "policies for subsidies and incentives", "integration with renewable energy sources for electricity generation"]</t>
+  </si>
+  <si>
+    <t>["Hydrogen production infrastructure", "availability of low-carbon hydrogen", "cost reductions in fuel cell systems", "durable policies to support adoption"]</t>
+  </si>
+  <si>
+    <t>["Availability and development of advanced lightweight materials", "efficient recycling processes", "industry-scale implementation"]</t>
+  </si>
+  <si>
+    <t>["Development and deployment of advanced vehicle technologies", "regulatory frameworks", "consumer acceptance"]</t>
+  </si>
+  <si>
+    <t>["Driver education", "effective training programs", "policy support", "incentive mechanisms", "encourage adoption of eco-driving practices"]</t>
+  </si>
+  <si>
+    <t>["Development and adoption of advanced aircraft technology", "global air traffic management optimization", "industry investments in research and development"]</t>
+  </si>
+  <si>
+    <t>["Availability of low-carbon energy", "advancements in fuel production technologies", "cost reductions", "policy support", "infrastructure for production and distribution"]</t>
+  </si>
+  <si>
+    <t>["Requires significant investments in HSR infrastructure", "policy support to limit competing air travel options", "integration of rail networks with existing transportation systems"]</t>
+  </si>
+  <si>
+    <t>["Availability of low-carbon fuels and energy", "infrastructure investments", "retrofitting capabilities for existing ships", "policy and regulatory support", "advances in fuel storage and safety technologies"]</t>
+  </si>
+  <si>
+    <t>["Availability of low-carbon electricity", "advancements in battery technology", "infrastructure for charging and maintenance", "supportive regulatory frameworks for the maritime industry"]</t>
+  </si>
+  <si>
+    <t>["Availability of low-carbon fuels", "advancements in propulsion and hull design technologies", "investments in port infrastructure", "regulatory support for energy efficiency and emissions reductions"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced technologies", "supportive regulatory frameworks", "investment in research and development", "alignment with global standards for emissions reduction and energy efficiency"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced fuel delivery systems", "supportive policy frameworks", "investment in R&amp;D for alternative reductants", "industry-wide adoption of optimized process controls and technologies"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced furnace designs", "supportive policies and incentives", "skilled workforce for installation and maintenance", "industry-wide adoption of energy-efficient technologies"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced heat recovery and pump technologies", "skilled workforce for installation and maintenance", "policy support for adoption of waste heat recovery systems"]</t>
+  </si>
+  <si>
+    <t>["Development and deployment of advanced process integration technologies", "skilled workforce training", "supportive policies to incentivize adoption"]</t>
+  </si>
+  <si>
+    <t>["Development of advanced comminution and ore sorting technologies", "availability of renewable energy sources for power generation", "policy support to incentivize adoption"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced drying/dewatering technologies", "skilled workforce for implementation", "supportive policies or incentives to offset initial costs"]</t>
+  </si>
+  <si>
+    <t>["Availability of recycling infrastructure", "advanced technologies for material separation and recovery", "supportive policies for incentivizing recycling practices"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced technologies like sensors and machine learning systems", "adequate digital infrastructure", "supportive policies for energy efficiency adoption"]</t>
+  </si>
+  <si>
+    <t>["Availability of renewable fuel infrastructure", "technology development for alternative fuel production", "supportive policies"]</t>
+  </si>
+  <si>
+    <t>["Availability of low-carbon electricity", "development of suitable anode materials", "infrastructure for large-scale electrification in steel production"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced heat recovery technologies", "skilled workforce for installation and operation", "supportive policies and funding incentives"]</t>
+  </si>
+  <si>
+    <t>["Development of advanced process technologies", "regulatory support for adoption", "workforce training", "sufficient financial incentives or subsidies to offset high initial costs"]</t>
+  </si>
+  <si>
+    <t>["Access to biomass resources", "skilled workforce for CHP system operation", "supportive policies to incentivize adoption of CHP systems"]</t>
+  </si>
+  <si>
+    <t>["Requires advancements in CCS and CCU technologies", "availability of low-GHG electricity", "supportive policies to incentivize industrial decarbonization"]</t>
+  </si>
+  <si>
+    <t>["Availability of clean energy for hydrogen production", "development of CCU technologies", "policies to support adoption"]</t>
+  </si>
+  <si>
+    <t>["Requires the development of CO2 transport and storage infrastructure", "supportive policy frameworks", "sufficient clean energy for capture processes", "incentives for adoption"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced materials", "supportive policies for circular economy", "stakeholder collaboration across supply chains", "investment in R&amp;D for lightweight materials", "high-efficiency design methods"]</t>
+  </si>
+  <si>
+    <t>["Availability of advanced manufacturing technologies", "workforce training", "supportive regulations", "access to materials for near-net shape casting"]</t>
+  </si>
+  <si>
+    <t>["Collaboration across supply chains", "advances in recycling and remanufacturing technologies", "supportive policy frameworks to incentivize adoption"]</t>
+  </si>
+  <si>
+    <t>["Effective coordination between industries, governments, and communities", "supportive policies and regulations", "development of recycling infrastructure", "data sharing platforms for material and energy flows"]</t>
+  </si>
+  <si>
+    <t>["Development and availability of alternative feedstocks", "regulatory support for material substitution", "investment in research and development for innovative concrete applications"]</t>
+  </si>
+  <si>
+    <t>["Availability of infrastructure for waste collection and recycling", "public awareness campaigns", "supportive policy frameworks"]</t>
+  </si>
+  <si>
+    <t>["Requires clear guidelines", "consumer education campaigns", "industry compliance with precise dosing recommendations"]</t>
+  </si>
+  <si>
+    <t>["Development of platforms and systems to facilitate product sharing", "stakeholder collaboration", "supportive policies to incentivize shared usage models"]</t>
+  </si>
+  <si>
+    <t>["Requires collaboration across material supply chains", "advancements in product design", "supportive policy frameworks to incentivize circular economy practices"]</t>
+  </si>
+  <si>
+    <t>["Development of advanced maintenance techniques", "effective policies to promote longer building lifespans", "education for construction professionals on durable practices"]</t>
+  </si>
+  <si>
+    <t>["Public awareness campaigns", "supportive policies", "integration of sustainability into business and governmental frameworks"]</t>
+  </si>
+  <si>
+    <t>["Implementation of policies and programs promoting sustainable consumption", "availability of alternatives to high-emission activities", "societal support for behavioral and lifestyle changes"]</t>
+  </si>
+  <si>
+    <t>["Requires improved governance", "clear land tenure policies", "funding for protected areas", "community participation in forest conservation efforts"]</t>
+  </si>
+  <si>
+    <t>["Requires funding for land restoration", "access to suitable species for planting", "local community engagement", "monitoring systems for ecosystem integrity and carbon sequestration"]</t>
+  </si>
+  <si>
+    <t>["Requires expertise in sustainable forestry", "investment in nurseries with adapted species", "supportive policies", "incentives to overcome economic barriers", "ensure accessibility for local stakeholders"]</t>
+  </si>
+  <si>
+    <t>["Effective governance frameworks", "access to research and technology for fire management", "community engagement", "alignment with regional legal and policy frameworks"]</t>
+  </si>
+  <si>
+    <t>["Strong policy frameworks", "financial incentives for conservation", "collaboration between governments", "local communities", "landowners to implement sustainable practices"]</t>
+  </si>
+  <si>
+    <t>["Requires strong governance", "financial support", "international cooperation", "policies to control land conversion drivers", "such as agriculture", "mining", "urban development"]</t>
+  </si>
+  <si>
+    <t>["Availability of funding", "collaboration among local and national stakeholders", "scientific research on optimal restoration practices", "policies to incentivize restoration efforts"]</t>
+  </si>
+  <si>
+    <t>["Effective integration of coastal climate mitigation policies", "marine spatial planning", "economic incentives to prioritize wetland conservation"]</t>
+  </si>
+  <si>
+    <t>["Requires long-term commitments", "supportive policies", "funding", "monitoring frameworks", "technical capacity", "to address drivers of degradation", "ensure restoration success"]</t>
+  </si>
+  <si>
+    <t>["Success depends on the availability of resources for monitoring and verification", "regional adaptation of practices", "addressing barriers such as soil saturation and permanence issues"]</t>
+  </si>
+  <si>
+    <t>["Availability of sustainably sourced biomass", "standardization of production methods", "monitoring systems", "incentives for scaling up biochar production and application"]</t>
+  </si>
+  <si>
+    <t>["Requires access to appropriate germplasm", "supportive policies", "extension systems", "credit access", "reforms in land tenure systems", "Adoption depends on aligning agroforestry practices to biophysical and socio-economic contexts"]</t>
+  </si>
+  <si>
+    <t>["Development and regulatory approval of feed additives, vaccines, and inhibitors", "regional adaptation of mitigation strategies", "overcoming barriers like costs, infrastructure, and public acceptance"]</t>
+  </si>
+  <si>
+    <t>["Adequate irrigation infrastructure", "training for farmers on advanced techniques", "access to slow-release fertilisers and biochar", "coordinated water management practices among neighboring farmers and regions"]</t>
+  </si>
+  <si>
+    <t>["Availability of training and technical support for farmers", "development of regional nutrient management roadmaps", "access to affordable fertilizers and inhibitors"]</t>
+  </si>
+  <si>
+    <t>["Development of cost-effective anaerobic digestion systems", "supportive policies for nitrification inhibitors", "region-specific training programs", "accessible financing for farmers"]</t>
+  </si>
+  <si>
+    <t>["Requires sustainable land management", "advanced bioenergy technology development", "infrastructure for carbon capture and storage", "global governance for trade and supply chains"]</t>
+  </si>
+  <si>
+    <t>["Implementation of integrated food-system policies", "financial incentives for sustainable agriculture", "awareness campaigns", "the development of local food systems to support dietary transitions"]</t>
+  </si>
+  <si>
+    <t>["Adequate infrastructure for food storage and transportation", "policy frameworks for waste reduction", "financial incentives", "widespread consumer education to change behaviors"]</t>
+  </si>
+  <si>
+    <t>["Requires sustainable forest management practices", "advanced wood processing technologies", "market demand for wood substitutes", "global cooperation to prevent resource exploitation"]</t>
+  </si>
+  <si>
+    <t>["Requires integrated spatial planning", "infrastructure development", "zoning regulations", "public transport investment"]</t>
+  </si>
+  <si>
+    <t>["Requires effective urban planning", "policy support for mixed land use", "investment in public transit infrastructure", "cooperation across municipal agencies"]</t>
+  </si>
+  <si>
+    <t>["High institutional capacity for cross-sector collaboration", "advanced GIS tools for spatial planning", "stakeholder engagement for co-design processes"]</t>
+  </si>
+  <si>
+    <t>["Requires grid upgrades", "supportive policies", "stakeholder cooperation", "financial incentives", "public awareness campaigns", "access to renewable energy", "advanced storage technologies is critical"]</t>
+  </si>
+  <si>
+    <t>['Sustainable forestry management', 'international carbon accounting standards', 'development of mass timber technologies', 'robust forest and urban land governance policies', 'incentivized afforestation practices']</t>
+  </si>
+  <si>
+    <t>["Availability of land for planting", "community participation", "funding for maintenance", "policies supporting urban greening initiatives"]</t>
+  </si>
+  <si>
+    <t>["Requires local government coordination", "community engagement", "urban planning integration", "adequate funding for infrastructure development and maintenance"]</t>
+  </si>
+  <si>
+    <t>["Requires integrated urban planning", "investment in active transport infrastructure", "collaboration between urban and transportation planners", "community engagement"]</t>
+  </si>
+  <si>
+    <t>["Requires institutional capacity", "governance", "cross-sectoral coordination", "public awareness campaigns", "needs infrastructure for decentralized waste treatment", "policies to promote circular economy practices"]</t>
+  </si>
+  <si>
+    <t>["Reduction in per capita car use", "increase in public transport ridership", "improved walkability index"]</t>
+  </si>
+  <si>
+    <t>["Increase in kilometers of bicycle and walking networks", "rise in active transport modal share", "reduction in car usage for short trips"]</t>
+  </si>
+  <si>
+    <t>["Increase in public transit ridership", "reduction in private vehicle kilometers traveled", "emissions reduction per passenger kilometer"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material intensity per unit output", "decrease in freight transport emissions", "increased adoption of circular economy practices"]</t>
+  </si>
+  <si>
+    <t>["Increase in shared mobility trips", "reduction in private vehicle kilometers traveled", "decreased transport-related emissions"]</t>
+  </si>
+  <si>
+    <t>["Reduction in commuter trips", "increase in teleworking adoption rates", "decreased transport-related emissions"]</t>
+  </si>
+  <si>
+    <t>["Increase in shared and public transport use", "reduction in private vehicle kilometers traveled", "decreased transport-related emissions"]</t>
+  </si>
+  <si>
+    <t>["Reduced freight distances", "increased vehicle carrying capacity", "improved fuel efficiency", "reduced operating costs"]</t>
+  </si>
+  <si>
+    <t>["Reduction in vehicle kilometers traveled (VMT) for shopping", "increase in online shopping adoption rates", "emissions reductions in freight logistics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in congestion", "improved fuel efficiency", "decreased transport-related emissions per vehicle kilometer", "increased accessibility for marginalized groups"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions from fuel lifecycle", "percentage of vehicle fleet using alternative fuels", "infrastructure deployment metrics"]</t>
+  </si>
+  <si>
+    <t>["Percentage of electric vehicles in the vehicle fleet", "reduction in GHG emissions per kilometer traveled", "availability of charging infrastructure"]</t>
+  </si>
+  <si>
+    <t>["Share of fuel cell vehicles in the vehicle fleet", "reduction in GHG emissions per kilometer", "deployment of hydrogen refueling stations", "cost parity with diesel vehicles"]</t>
+  </si>
+  <si>
+    <t>["Reduction in vehicle mass", "improvement in fuel efficiency (km/l)", "lifecycle GHG emissions avoided", "share of lightweighted vehicles in the fleet"]</t>
+  </si>
+  <si>
+    <t>["Improvements in fuel economy (km/l)", "reduction in GHG emissions per km", "share of energy-efficient vehicles in fleets", "fuel cost savings"]</t>
+  </si>
+  <si>
+    <t>["Percentage reduction in fuel consumption", "GHG emissions per vehicle", "number of drivers trained in eco-driving", "adherence to eco-driving practices among trained drivers"]</t>
+  </si>
+  <si>
+    <t>["Percentage reduction in fuel consumption per flight", "improvement in navigation efficiency", "adoption rate of advanced aircraft designs"]</t>
+  </si>
+  <si>
+    <t>["Adoption rates of SAFs", "lifecycle emissions reductions", "advancements in fuel production technologies"]</t>
+  </si>
+  <si>
+    <t>["Reduction in domestic and regional air travel demand", "increase in HSR ridership", "measurable reductions in transportation sector GHG emissions"]</t>
+  </si>
+  <si>
+    <t>["Adoption rate of alternative fuels", "emissions reductions achieved (tank-to-wake and well-to-wake)", "advancements in bunkering and storage infrastructure"]</t>
+  </si>
+  <si>
+    <t>["Reduction in lifecycle emissions of vessels", "number of electric and hybrid-electric ships in operation", "improvements in port infrastructure to support electric propulsion systems"]</t>
+  </si>
+  <si>
+    <t>["Reduction in shipping emissions", "adoption rate of energy-efficient technologies", "operational measures", "number of retrofitted vessels", "efficiency improvements in port operations"]</t>
+  </si>
+  <si>
+    <t>["Reduction in industrial GHG emissions", "adoption rates of heat and energy recovery technologies", "energy intensity improvements in key industries", "recycling rates"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions from heating in steel production", "energy intensity improvements", "increased adoption rates of pulverized coal injection and alternative fuels", "reduced production of hazardous wastes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy intensity", "GHG emissions", "hazardous waste production", "increased adoption of advanced furnaces", "process controls"]</t>
+  </si>
+  <si>
+    <t>["Increase in waste heat recovery rate", "reduction in energy intensity", "percentage of heat reused through high-efficiency systems"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy consumption per unit of steel", "increase in process coupling efficiency", "reduction in GHG emissions per ton of steel produced"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy consumption per ton of ore processed", "improvement in ore recovery ratio", "reduction in GHG emissions from mining operations"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy consumption per unit of output", "percentage improvement in drying efficiency", "reduction in GHG emissions from manufacturing processes"]</t>
+  </si>
+  <si>
+    <t>["Recycling rates by material type", "reduction in energy consumption for material production", "decrease in landfill waste volumes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy use", "cost savings per production cycle", "percentage improvement in process efficiency"]</t>
+  </si>
+  <si>
+    <t>["Reduction in CO2 emissions", "increased adoption rate of renewable fuels", "reduction in the carbon intensity of industrial processes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in emissions per ton of steel produced", "increase in the share of electrified processes", "energy savings in production stages"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy consumption per ton of product", "increase in waste energy recovery rates", "decrease in GHG emissions intensity in industrial processes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy use per unit of production", "lower emissions per ton of material produced", "increased adoption rate of advanced technologies", "improved process efficiency metrics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in energy intensity per ton of paper", "decrease in direct and indirect CO2 emissions", "increase in on-site electricity production through CHP systems"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions from industrial processes", "increase in the use of low-carbon feedstocks", "the number of CCS/CCU projects implemented"]</t>
+  </si>
+  <si>
+    <t>["Quantity of CO2 captured and reused", "reduction in emissions per ton of product", "market penetration of CCU-derived products"]</t>
+  </si>
+  <si>
+    <t>["Amount of CO2 captured and stored annually", "percentage reduction in industrial emissions", "operational capacity of CCS projects globally"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material usage per product", "increase in product lifespan", "percentage of materials recovered and reused", "reduction in GHG emissions from production processes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material waste", "increase in production yield", "reduction in GHG emissions per unit of material produced"]</t>
+  </si>
+  <si>
+    <t>["Percentage of materials recovered and reused", "reduction in production waste", "decrease in GHG emissions per unit of product lifecycle"]</t>
+  </si>
+  <si>
+    <t>["Reduction in virgin material use", "GHG emissions avoided through CE practices", "increase in recycling rates", "number of industrial symbiosis networks implemented", "resource recovery metrics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in clinker-to-cement ratio", "lower CO2 emissions per tonne of cement", "increased adoption of alternative materials in cement production"]</t>
+  </si>
+  <si>
+    <t>["Reduction in food waste percentage", "increased recycling rates", "reduced greenhouse gas emissions from waste management"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material waste", "increased adherence to dosing guidelines", "measurable decreases in associated emissions"]</t>
+  </si>
+  <si>
+    <t>["Number of shared product-service systems implemented", "reduction in material demand per capita", "decrease in GHG emissions from product manufacturing"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material use per product", "increase in product lifespan", "rate of reuse and repair", "reduction in GHG emissions from material production and waste"]</t>
+  </si>
+  <si>
+    <t>["Increase in the average lifespan of buildings and infrastructure", "reduction in cement demand per capita", "overall CO2 emissions reductions in cement production"]</t>
+  </si>
+  <si>
+    <t>["Reduction in material and energy intensity per capita", "decrease in waste generation rates", "improvement in recycling and reuse statistics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in demand for high-emission products and services", "decreased industrial emissions linked to product use", "increased adoption of sustainable consumption practices"]</t>
+  </si>
+  <si>
+    <t>["Reduction in deforestation rates", "increased forest cover", "the amount of GHG emissions avoided per year"]</t>
+  </si>
+  <si>
+    <t>["Area of land reforested or afforested", "carbon sequestration rates", "improvement in biodiversity indices", "ecosystem service metrics such as water regulation and soil quality"]</t>
+  </si>
+  <si>
+    <t>["Increase in forest carbon stocks", "reduction in GHG emissions", "improvements in biodiversity indicators", "reduction in soil erosion and water-related issues"]</t>
+  </si>
+  <si>
+    <t>["Reduction in frequency and intensity of uncontrolled wildfires", "Area managed with prescribed burns", "Reduction in GHG emissions from fires", "Improvement in biodiversity and soil health metrics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in conversion rates of grasslands", "increase in soil organic carbon levels", "measurable reduction in GHG emissions from targeted areas"]</t>
+  </si>
+  <si>
+    <t>["Reduction in peatland conversion rates", "avoided emissions per hectare", "improvements in biodiversity and water quality metrics"]</t>
+  </si>
+  <si>
+    <t>["Area of coastal wetlands preserved", "GHG emissions avoided from biomass and soil carbon loss", "improvements in biodiversity metrics", "ecosystem resilience"]</t>
+  </si>
+  <si>
+    <t>["Area of wetlands restored", "carbon sequestration rates", "biodiversity recovery metrics", "reduction in storm damage costs", "water quality improvements"]</t>
+  </si>
+  <si>
+    <t>["Increase in soil organic carbon", "reduction in GHG emissions", "improvement in agricultural productivity", "biodiversity enhancements"]</t>
+  </si>
+  <si>
+    <t>["Carbon sequestration rates", "reduction in soil N2O emissions", "crop yield improvements", "displacement of fossil fuel use through pyrolysis gases"]</t>
+  </si>
+  <si>
+    <t>["Carbon sequestration rates (above and below ground)", "improved soil health metrics", "increase in farmer income", "reduction in soil erosion", "adoption rates of agroforestry systems"]</t>
+  </si>
+  <si>
+    <t>["Reduction in CH4 emissions per animal", "adoption rates of improved feeding practices", "increase in production efficiency per unit of livestock product"]</t>
+  </si>
+  <si>
+    <t>["Reduction in CH4 and N2O emissions per hectare", "increased water use efficiency", "yield stability during droughts", "adoption rate of improved rice cultivation techniques"]</t>
+  </si>
+  <si>
+    <t>["Reduction in N2O emissions", "improvement in crop yields", "increase in soil carbon sequestration", "reduction in fertilizer use per hectare"]</t>
+  </si>
+  <si>
+    <t>["Reduction in CH4 and N2O emissions from manure storage", "increased adoption of anaerobic digestion systems", "improved nitrogen use efficiency", "enhanced biogas production"]</t>
+  </si>
+  <si>
+    <t>["Amount of carbon removed through BECCS (in GtCO2 per year)", "total energy produced from bioenergy", "land restored for biomass production", "GHG emissions reduction from displaced fossil fuel use"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions from food production", "reduction in land use for livestock", "increase in plant-based food consumption", "improvement in public health metrics related to diet-related diseases"]</t>
+  </si>
+  <si>
+    <t>["Reduction in food waste percentages at consumer and business levels", "decrease in land used for agricultural production", "measurable GHG emission reductions across the food supply chain"]</t>
+  </si>
+  <si>
+    <t>["Increased use of wood products in construction", "reduction in GHG emissions from material substitution", "increase in recycled wood product utilization rates"]</t>
+  </si>
+  <si>
+    <t>['Reduction in vehicle miles traveled', 'increase in public transport usage', 'percentage of urban areas with mixed-use development', 'lower per capita energy use in urban areas']</t>
+  </si>
+  <si>
+    <t>["Reduction in VMT", "increase in public transit ridership", "decrease in transport-related GHG emissions", "improved accessibility to jobs and housing"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions per capita", "adoption rates of district heating/cooling systems", "proportion of urban population with access to green areas"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions per kWh", "increase in renewable energy penetration", "adoption rates of EVs and heat pumps", "improved urban air quality"]</t>
+  </si>
+  <si>
+    <t>["Reduction in embodied carbon in construction", "number of mid-rise urban buildings using engineered timber", "carbon sequestration capacity of urban timber infrastructure", "improvement in sustainable forestry practices"]</t>
+  </si>
+  <si>
+    <t>["Increase in urban tree cover percentage", "reduction in urban heat island effect", "amount of carbon sequestered", "reduction in building energy use", "improvement in air quality metrics"]</t>
+  </si>
+  <si>
+    <t>["Reduction in building energy consumption", "increase in urban green coverage", "stormwater retention rates", "increased active transportation use (cycling/walking)", "improved thermal comfort"]</t>
+  </si>
+  <si>
+    <t>["Reduction in vehicle miles traveled (VMT)", "increase in walking and biking trips", "reduction in urban GHG emissions", "improved accessibility to essential services"]</t>
+  </si>
+  <si>
+    <t>["Reduction in waste generation per capita", "increase in recycling and composting rates", "reduction in CH4 emissions from waste", "employment opportunities created in waste management"]</t>
+  </si>
+  <si>
+    <t>["Improved urban livability", "better public health outcomes", "reduced GHG emissions"]</t>
+  </si>
+  <si>
+    <t>["Improved public health", "reduced urban congestion", "lower transport-related GHG emissions", "enhanced quality of urban life"]</t>
+  </si>
+  <si>
+    <t>["Enhanced urban livability", "reduced traffic congestion", "improved public health", "significant reductions in transport-related greenhouse gas emissions"]</t>
+  </si>
+  <si>
+    <t>["Improved resource efficiency", "lower environmental footprint", "potential for reduced transport emissions"]</t>
+  </si>
+  <si>
+    <t>["Enhanced urban mobility", "reduced traffic congestion", "lower transport emissions", "increased system efficiency"]</t>
+  </si>
+  <si>
+    <t>["Reduced traffic congestion", "improved air quality", "enhanced work-life balance", "lower transport emissions"]</t>
+  </si>
+  <si>
+    <t>["Enhanced urban livability", "reduced congestion", "improved air quality", "significant advancements in transport efficiency"]</t>
+  </si>
+  <si>
+    <t>["Reduced operating costs", "improved corporate image", "enhanced transport infrastructure utilisation", "potential air quality improvement"]</t>
+  </si>
+  <si>
+    <t>["Improved urban mobility", "reduced shopping-related travel emissions", "enhanced convenience for consumers"]</t>
+  </si>
+  <si>
+    <t>["Enhanced road safety", "reduced traffic congestion", "increased accessibility for underserved populations", "optimization of transport systems for environmental and societal benefit"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "improved air quality", "energy diversification", "increased resilience in transportation systems"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "improved urban air quality", "decreased reliance on fossil fuels", "greater energy security"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "improved air quality", "energy diversification", "advancement of clean technologies for transportation"]</t>
+  </si>
+  <si>
+    <t>['Reduced GHG emissions', 'enhanced fuel efficiency', 'improved vehicle performance', 'contribution to a circular economy through advanced recycling']</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "enhanced fuel efficiency", "lower operating costs", "improved air quality"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "enhanced fuel efficiency", "improved road safety", "lower transport costs"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "enhanced operational efficiency", "strengthened energy security in aviation"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in aviation emissions", "improved energy security", "progress toward net-zero aviation operations"]</t>
+  </si>
+  <si>
+    <t>["Reduces aviation emissions", "improves regional connectivity", "decreases transportation-related air pollution", "enhances public transportation networks"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in maritime emissions", "improved air quality", "progress toward global decarbonization goals", "reduced reliance on fossil fuels in the shipping industry"]</t>
+  </si>
+  <si>
+    <t>["Significant reduction in maritime sector emissions", "Improved air quality in coastal and port regions", "Decreased reliance on fossil fuels", "Promotion of innovation in clean transportation technologies"]</t>
+  </si>
+  <si>
+    <t>["Reduction in maritime emissions", "improved air and water quality", "increased energy security", "enhanced innovation in sustainable shipping technologies"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in industrial emissions", "improved resource efficiency", "enhanced energy security", "increased sustainability in manufacturing and construction sectors"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in emissions and energy use in steel manufacturing", "improved air quality", "enhanced energy security", "more sustainable industrial practices"]</t>
+  </si>
+  <si>
+    <t>["Significant improvements in industrial energy efficiency", "reduced emissions", "cost savings for manufacturers", "enhanced air quality"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in industrial energy consumption and GHG emissions", "enhanced energy security", "cost savings for manufacturers", "reduced environmental waste"]</t>
+  </si>
+  <si>
+    <t>["Improved energy efficiency", "reduced emissions", "cost savings for manufacturers", "enhanced competitiveness of the steel industry in global markets"]</t>
+  </si>
+  <si>
+    <t>["Improved energy efficiency in mining", "reduced operational costs", "decreased environmental footprint of mining activities", "enhanced resource utilization"]</t>
+  </si>
+  <si>
+    <t>["Increased energy efficiency", "reduced operational costs", "lower emissions", "enhanced sustainability in industrial processes"]</t>
+  </si>
+  <si>
+    <t>["Reduces reliance on virgin material extraction", "lowers industrial energy demand", "mitigates GHG emissions", "supports sustainable production practices"]</t>
+  </si>
+  <si>
+    <t>["Enhanced energy efficiency", "reduced operational costs", "improved industrial competitiveness", "support for decarbonization goals"]</t>
+  </si>
+  <si>
+    <t>["Reduced dependence on fossil fuels", "improved energy security", "mitigation of air pollution", "contributing to global emission reduction targets"]</t>
+  </si>
+  <si>
+    <t>["Reduced reliance on fossil fuels", "improved air quality", "enhanced global competitiveness of steel manufacturers"]</t>
+  </si>
+  <si>
+    <t>["Enhances energy efficiency", "reduces emissions", "lowers operational costs", "improves competitiveness of the industrial sector in global markets"]</t>
+  </si>
+  <si>
+    <t>["Enhanced energy efficiency", "significant emissions reductions", "cost savings for industries", "increased competitiveness in global markets", "improved environmental sustainability"]</t>
+  </si>
+  <si>
+    <t>["Improved energy efficiency", "reduced emissions", "enhanced competitiveness of the pulp and paper industry", "long-term cost savings for manufacturers"]</t>
+  </si>
+  <si>
+    <t>["Enhanced industrial sustainability", "reduced dependence on fossil fuels", "advancement of circular economy principles", "mitigation of climate change impacts"]</t>
+  </si>
+  <si>
+    <t>["Reduction in GHG emissions", "enhanced energy security", "development of sustainable industries"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in GHG emissions", "mitigation of climate change effects", "increased energy security through sustainable industrial practices"]</t>
+  </si>
+  <si>
+    <t>["Reduced environmental footprint", "lower production costs", "improved resource efficiency", "enhanced sustainability of industrial processes"]</t>
+  </si>
+  <si>
+    <t>["Significant reduction in material and energy use", "enhanced production efficiency", "reduced emissions", "improved sustainability across industrial supply chains"]</t>
+  </si>
+  <si>
+    <t>["Reduction in raw material demand", "improved environmental sustainability", "decreased emissions", "enhanced industrial efficiency"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in resource extraction, energy use, and emissions", "enhanced regional development through eco-industrial parks", "broader adoption of sustainable practices across industries and urban areas"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "enhanced resource efficiency", "lower energy consumption in cement production", "improved environmental quality in cement manufacturing regions"]</t>
+  </si>
+  <si>
+    <t>["Reduced environmental burden", "enhanced resource efficiency", "improved urban livability", "cost savings in waste management systems"]</t>
+  </si>
+  <si>
+    <t>["Reduced industrial emissions", "lower resource consumption", "cost savings for consumers and industries", "improved efficiency across the supply chain"]</t>
+  </si>
+  <si>
+    <t>["Reduction in resource use and emissions", "cost savings for consumers", "increased accessibility to products", "fostering a circular economy through more efficient use of materials"]</t>
+  </si>
+  <si>
+    <t>["Significant emissions reductions", "resource conservation", "cost savings for consumers", "strengthened circular economy practices"]</t>
+  </si>
+  <si>
+    <t>["Reduction in demand for new concrete and cement production", "reduced emissions", "enhanced resource efficiency", "increased affordability and sustainability of infrastructure"]</t>
+  </si>
+  <si>
+    <t>["Enhances societal well-being", "reducing overconsumption", "lowering environmental impacts", "fostering long-term sustainability in resource use", "industrial processes"]</t>
+  </si>
+  <si>
+    <t>["Reduction in global GHG emissions", "improved resource efficiency", "enhanced sustainability in consumption patterns", "reduced strain on environmental resources"]</t>
+  </si>
+  <si>
+    <t>["Preserves biodiversity", "enhances ecosystem services", "improves air and water quality", "contributes to climate stabilization", "sustainable development"]</t>
+  </si>
+  <si>
+    <t>["Increased carbon sequestration", "improved biodiversity", "enhanced ecosystem resilience", "better water regulation", "soil stabilization", "support for local communities through sustainable resource use"]</t>
+  </si>
+  <si>
+    <t>["Improved forest health and resilience", "enhanced carbon sequestration", "biodiversity conservation", "increased ecosystem services like water and soil regulation"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "improved biodiversity conservation", "prevention of soil erosion", "enhanced land productivity", "reduced risks to life and property from uncontrolled wildfires"]</t>
+  </si>
+  <si>
+    <t>["Preserves ecosystem services", "enhances biodiversity", "supports climate resilience", "provides sustainable livelihoods for communities dependent on grasslands"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "enhanced biodiversity", "improved water regulation", "decreased fire-related health hazards"]</t>
+  </si>
+  <si>
+    <t>["Significant reductions in CO2 emissions", "improved biodiversity", "enhanced water regulation", "reduced flooding risks", "increased resilience to climate change"]</t>
+  </si>
+  <si>
+    <t>["Increased carbon sequestration", "enhanced resilience to climate impacts", "improved biodiversity", "better water quality", "greater protection against flooding and storm surges"]</t>
+  </si>
+  <si>
+    <t>["Enhanced ecosystem resilience", "improved carbon sequestration", "protection against sea-level rise and storms", "increased biodiversity", "strengthened coastal livelihoods", "food security"]</t>
+  </si>
+  <si>
+    <t>["Enhanced soil health", "improved water retention", "increased crop yields", "greater biodiversity", "reduced erosion", "resilience to climate change in agricultural and grassland ecosystems"]</t>
+  </si>
+  <si>
+    <t>["Improved agricultural productivity", "enhanced soil resilience to climate change", "reduced pollution", "long-term carbon storage in soils", "contributing to global climate goals"]</t>
+  </si>
+  <si>
+    <t>["Enhanced land productivity", "improved livelihoods", "increased carbon storage", "better water quality", "resilience to climate change"]</t>
+  </si>
+  <si>
+    <t>["Reduction in global agricultural methane emissions", "improved livestock productivity", "enhanced food security", "particularly in regions with high agricultural dependence"]</t>
+  </si>
+  <si>
+    <t>["Reduced greenhouse gas emissions", "improved water use efficiency", "enhanced drought resilience", "increased farm income", "more sustainable agricultural practices", "contributing to food security"]</t>
+  </si>
+  <si>
+    <t>["Contributes to climate mitigation", "improves food and nutrition security", "enhances environmental sustainability", "supports long-term agricultural productivity"]</t>
+  </si>
+  <si>
+    <t>["Reduces greenhouse gas emissions", "improves local water and air quality", "enhances soil health", "supports food security", "provides renewable energy through biogas production"]</t>
+  </si>
+  <si>
+    <t>["Enhanced energy security", "reduced GHG emissions", "restored degraded lands", "improved air and water quality", "biodiversity conservation"]</t>
+  </si>
+  <si>
+    <t>["Improved public health outcomes", "reduced environmental pressures (e.g., deforestation, biodiversity loss)", "strengthened food security through sustainable practices"]</t>
+  </si>
+  <si>
+    <t>["Enhances food security", "reduces environmental stress on water and land resources", "supports poverty alleviation", "contributes to achieving SDG 12 for sustainable consumption and production patterns"]</t>
+  </si>
+  <si>
+    <t>["Reduces emissions from traditional material production", "enhances carbon sequestration", "supports sustainable forest industries", "provides economic opportunities in rural and forested areas"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions", "improved public health", "better urban livability", "reduced resource consumption", "preservation of land for agriculture and forestry"]</t>
+  </si>
+  <si>
+    <t>["Reduces GHG emissions", "improves air quality", "enhances urban livability", "fosters more sustainable urban growth patterns"]</t>
+  </si>
+  <si>
+    <t>["Enhanced livability", "improved public health", "reduced energy use", "increased resilience to climate impacts", "promotion of green economic growth"]</t>
+  </si>
+  <si>
+    <t>["Enhances energy security", "reduces urban air pollution", "improves public health", "supports sustainable urban development through renewable energy and electrification"]</t>
+  </si>
+  <si>
+    <t>["Reduced GHG emissions from construction", "enhanced carbon storage in urban environments", "sustainable urbanization", "improved resource efficiency", "reduced pressure on natural ecosystems"]</t>
+  </si>
+  <si>
+    <t>["Enhanced urban livability", "improved public health", "reduced energy consumption", "increased biodiversity", "greater resilience to climate change impacts"]</t>
+  </si>
+  <si>
+    <t>["Enhanced urban livability", "reduced urban heat island effects", "improved public health", "better stormwater management", "increased biodiversity in urban areas"]</t>
+  </si>
+  <si>
+    <t>["Reduces urban energy use", "improves public health", "enhances urban livability", "fosters community engagement through better connectivity and accessibility"]</t>
+  </si>
+  <si>
+    <t>["Improved urban livability", "reduction in landfill emissions", "enhanced resource efficiency", "economic growth through job creation in the waste management sector"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2396,36 +2394,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D975116D-6FA8-43BD-BEAC-648ED712F7D0}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{E9328F65-C0A6-4011-B5D3-626A5546BE07}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2654,9 +2654,6 @@
     <text xml:space="preserve">Every co-benefit has a value 1
 </text>
   </threadedComment>
-  <threadedComment ref="R1" dT="2024-11-25T07:57:17.62" personId="{3B71A11A-A90E-4022-AEAC-3FBF1647287A}" id="{9D5EEA5E-CA47-4003-91AF-82CBBFC75B37}">
-    <text>Needs to be an array of strings [””,””,””]</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2667,8 +2664,8 @@
   </sheetPr>
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2687,8 +2684,8 @@
     <col min="16" max="16" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="115.36328125" customWidth="1"/>
-    <col min="19" max="19" width="81" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="148.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="95.7265625" customWidth="1"/>
+    <col min="20" max="20" width="121.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -2717,13 +2714,13 @@
         <v>360</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>747</v>
+        <v>508</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>748</v>
+        <v>509</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>367</v>
@@ -2794,19 +2791,19 @@
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
@@ -2850,19 +2847,19 @@
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="41.5" customHeight="1">
@@ -2906,19 +2903,19 @@
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1">
@@ -2962,19 +2959,19 @@
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
@@ -3018,19 +3015,19 @@
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="1" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1">
@@ -3074,19 +3071,19 @@
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="3" t="s">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
@@ -3130,22 +3127,22 @@
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="38.5" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>376</v>
       </c>
@@ -3186,19 +3183,19 @@
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1">
@@ -3242,19 +3239,19 @@
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1">
@@ -3298,19 +3295,19 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R11" s="10" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="T11" s="10" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
@@ -3354,19 +3351,19 @@
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="T12" s="10" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1">
@@ -3410,19 +3407,19 @@
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="T13" s="10" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1">
@@ -3466,19 +3463,19 @@
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="T14" s="10" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1">
@@ -3522,19 +3519,19 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="25.5" customHeight="1">
@@ -3578,19 +3575,19 @@
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="T16" s="10" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1">
@@ -3634,19 +3631,19 @@
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="3" t="s">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R17" s="10" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="T17" s="10" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1">
@@ -3690,19 +3687,19 @@
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="T18" s="10" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="68" customHeight="1">
@@ -3746,19 +3743,19 @@
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R19" s="10" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="31.5" customHeight="1">
@@ -3802,19 +3799,19 @@
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="T20" s="10" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="37.5" customHeight="1">
@@ -3858,19 +3855,19 @@
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R21" s="10" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="T21" s="10" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="50" customHeight="1">
@@ -3914,19 +3911,19 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="T22" s="10" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="41.5" customHeight="1">
@@ -3970,19 +3967,19 @@
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R23" s="10" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1">
@@ -4026,19 +4023,19 @@
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="T24" s="10" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1">
@@ -4082,19 +4079,19 @@
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R25" s="10" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="T25" s="10" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1">
@@ -4138,19 +4135,19 @@
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="T26" s="10" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1">
@@ -4194,19 +4191,19 @@
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R27" s="10" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="T27" s="10" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1">
@@ -4250,19 +4247,19 @@
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1">
@@ -4306,19 +4303,19 @@
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R29" s="10" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="T29" s="10" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="62.5">
@@ -4362,19 +4359,19 @@
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R30" s="10" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="T30" s="10" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="75">
@@ -4418,19 +4415,19 @@
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R31" s="10" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="T31" s="10" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="62.5">
@@ -4474,19 +4471,19 @@
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R32" s="10" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="62.5">
@@ -4530,19 +4527,19 @@
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="T33" s="10" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="50">
@@ -4586,19 +4583,19 @@
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R34" s="10" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="T34" s="10" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="50">
@@ -4642,19 +4639,19 @@
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R35" s="10" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="T35" s="10" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="87.5">
@@ -4698,19 +4695,19 @@
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="T36" s="10" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="50">
@@ -4754,19 +4751,19 @@
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R37" s="10" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="S37" s="10" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="T37" s="10" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="100">
@@ -4810,19 +4807,19 @@
       </c>
       <c r="O38" s="9"/>
       <c r="P38" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R38" s="10" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="S38" s="10" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="T38" s="10" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="62.5">
@@ -4866,19 +4863,19 @@
       </c>
       <c r="O39" s="9"/>
       <c r="P39" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R39" s="10" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="S39" s="10" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="T39" s="10" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="87.5">
@@ -4922,19 +4919,19 @@
       </c>
       <c r="O40" s="9"/>
       <c r="P40" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R40" s="10" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="S40" s="10" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="T40" s="10" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="75">
@@ -4978,19 +4975,19 @@
       </c>
       <c r="O41" s="9"/>
       <c r="P41" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R41" s="10" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="S41" s="10" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="T41" s="10" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="87.5">
@@ -5034,19 +5031,19 @@
       </c>
       <c r="O42" s="9"/>
       <c r="P42" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R42" s="10" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="S42" s="10" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="T42" s="10" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="75">
@@ -5090,19 +5087,19 @@
       </c>
       <c r="O43" s="9"/>
       <c r="P43" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R43" s="10" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="S43" s="10" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="T43" s="10" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="100">
@@ -5146,19 +5143,19 @@
       </c>
       <c r="O44" s="9"/>
       <c r="P44" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R44" s="10" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="S44" s="10" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="T44" s="10" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="87.5">
@@ -5202,19 +5199,19 @@
       </c>
       <c r="O45" s="9"/>
       <c r="P45" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R45" s="10" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="S45" s="10" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="T45" s="10" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="75">
@@ -5258,19 +5255,19 @@
       </c>
       <c r="O46" s="9"/>
       <c r="P46" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="S46" s="10" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="T46" s="10" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="62.5">
@@ -5314,19 +5311,19 @@
       </c>
       <c r="O47" s="9"/>
       <c r="P47" s="3" t="s">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="S47" s="10" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="T47" s="10" t="s">
-        <v>709</v>
+        <v>714</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="62.5">
@@ -5370,19 +5367,19 @@
       </c>
       <c r="O48" s="9"/>
       <c r="P48" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R48" s="10" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="S48" s="10" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="T48" s="10" t="s">
-        <v>710</v>
+        <v>715</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="62.5">
@@ -5426,19 +5423,19 @@
       </c>
       <c r="O49" s="9"/>
       <c r="P49" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R49" s="10" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="S49" s="10" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="T49" s="10" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="62.5">
@@ -5482,19 +5479,19 @@
       </c>
       <c r="O50" s="9"/>
       <c r="P50" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q50" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R50" s="10" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="S50" s="10" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="T50" s="10" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="75">
@@ -5538,19 +5535,19 @@
       </c>
       <c r="O51" s="9"/>
       <c r="P51" s="3" t="s">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R51" s="10" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="S51" s="10" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="T51" s="10" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="87.5">
@@ -5594,19 +5591,19 @@
       </c>
       <c r="O52" s="9"/>
       <c r="P52" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R52" s="10" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="S52" s="10" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="T52" s="10" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="75">
@@ -5650,19 +5647,19 @@
       </c>
       <c r="O53" s="9"/>
       <c r="P53" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="S53" s="10" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="T53" s="10" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="75">
@@ -5706,19 +5703,19 @@
       </c>
       <c r="O54" s="9"/>
       <c r="P54" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R54" s="10" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="S54" s="10" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="T54" s="10" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="75">
@@ -5762,19 +5759,19 @@
       </c>
       <c r="O55" s="9"/>
       <c r="P55" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="T55" s="10" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="75">
@@ -5818,19 +5815,19 @@
       </c>
       <c r="O56" s="9"/>
       <c r="P56" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R56" s="10" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="S56" s="10" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="T56" s="10" t="s">
-        <v>718</v>
+        <v>723</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="75">
@@ -5874,19 +5871,19 @@
       </c>
       <c r="O57" s="9"/>
       <c r="P57" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R57" s="10" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="S57" s="10" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="T57" s="10" t="s">
-        <v>719</v>
+        <v>724</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="62.5">
@@ -5930,19 +5927,19 @@
       </c>
       <c r="O58" s="9"/>
       <c r="P58" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R58" s="10" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="S58" s="10" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="T58" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="87.5">
@@ -5986,19 +5983,19 @@
       </c>
       <c r="O59" s="9"/>
       <c r="P59" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R59" s="10" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="S59" s="10" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="T59" s="10" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="75">
@@ -6042,19 +6039,19 @@
       </c>
       <c r="O60" s="9"/>
       <c r="P60" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R60" s="10" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="S60" s="10" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="T60" s="10" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="87.5">
@@ -6098,19 +6095,19 @@
       </c>
       <c r="O61" s="9"/>
       <c r="P61" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q61" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R61" s="10" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="S61" s="10" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="T61" s="10" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
     </row>
     <row r="62" spans="1:20" ht="112.5">
@@ -6154,19 +6151,19 @@
       </c>
       <c r="O62" s="9"/>
       <c r="P62" s="3" t="s">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R62" s="10" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="S62" s="10" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="T62" s="10" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="75">
@@ -6210,19 +6207,19 @@
       </c>
       <c r="O63" s="9"/>
       <c r="P63" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R63" s="10" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="S63" s="10" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="T63" s="10" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="75">
@@ -6266,19 +6263,19 @@
       </c>
       <c r="O64" s="9"/>
       <c r="P64" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q64" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R64" s="10" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="S64" s="10" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="T64" s="10" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="75">
@@ -6322,19 +6319,19 @@
       </c>
       <c r="O65" s="9"/>
       <c r="P65" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q65" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R65" s="10" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="S65" s="10" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="T65" s="10" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
     </row>
     <row r="66" spans="1:20" ht="75">
@@ -6378,19 +6375,19 @@
       </c>
       <c r="O66" s="9"/>
       <c r="P66" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R66" s="10" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="S66" s="10" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="T66" s="10" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
     </row>
     <row r="67" spans="1:20" ht="87.5">
@@ -6434,19 +6431,19 @@
       </c>
       <c r="O67" s="9"/>
       <c r="P67" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q67" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R67" s="10" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="S67" s="10" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="T67" s="10" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="87.5">
@@ -6490,19 +6487,19 @@
       </c>
       <c r="O68" s="9"/>
       <c r="P68" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R68" s="10" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="S68" s="10" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="T68" s="10" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="100">
@@ -6546,19 +6543,19 @@
       </c>
       <c r="O69" s="9"/>
       <c r="P69" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R69" s="10" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="S69" s="10" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="T69" s="10" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="75">
@@ -6602,19 +6599,19 @@
       </c>
       <c r="O70" s="9"/>
       <c r="P70" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R70" s="10" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="S70" s="10" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
       <c r="T70" s="10" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
     </row>
     <row r="71" spans="1:20" ht="100">
@@ -6658,19 +6655,19 @@
       </c>
       <c r="O71" s="9"/>
       <c r="P71" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q71" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R71" s="10" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="S71" s="10" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="T71" s="10" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="62.5">
@@ -6714,19 +6711,19 @@
       </c>
       <c r="O72" s="9"/>
       <c r="P72" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q72" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R72" s="10" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="S72" s="10" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="T72" s="10" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
     </row>
     <row r="73" spans="1:20" ht="62.5">
@@ -6770,19 +6767,19 @@
       </c>
       <c r="O73" s="9"/>
       <c r="P73" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q73" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R73" s="10" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="S73" s="10" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="T73" s="10" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="87.5">
@@ -6826,19 +6823,19 @@
       </c>
       <c r="O74" s="9"/>
       <c r="P74" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q74" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R74" s="10" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="S74" s="10" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="T74" s="10" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
     </row>
     <row r="75" spans="1:20" ht="75">
@@ -6882,19 +6879,19 @@
       </c>
       <c r="O75" s="9"/>
       <c r="P75" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q75" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R75" s="10" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="S75" s="10" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="T75" s="10" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="87.5">
@@ -6938,19 +6935,19 @@
       </c>
       <c r="O76" s="9"/>
       <c r="P76" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q76" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R76" s="10" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="S76" s="10" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="T76" s="10" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
     </row>
     <row r="77" spans="1:20" ht="75">
@@ -6994,19 +6991,19 @@
       </c>
       <c r="O77" s="9"/>
       <c r="P77" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q77" s="3" t="s">
         <v>24</v>
       </c>
       <c r="R77" s="10" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="S77" s="10" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="T77" s="10" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
     </row>
     <row r="78" spans="1:20" ht="62.5">
@@ -7050,19 +7047,19 @@
       </c>
       <c r="O78" s="9"/>
       <c r="P78" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q78" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R78" s="10" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="S78" s="10" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="T78" s="10" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
     </row>
     <row r="79" spans="1:20" ht="75">
@@ -7106,19 +7103,19 @@
       </c>
       <c r="O79" s="9"/>
       <c r="P79" s="3" t="s">
-        <v>745</v>
+        <v>506</v>
       </c>
       <c r="Q79" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R79" s="10" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="S79" s="10" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="T79" s="10" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
     </row>
     <row r="80" spans="1:20" ht="75">
@@ -7162,19 +7159,19 @@
       </c>
       <c r="O80" s="9"/>
       <c r="P80" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q80" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R80" s="10" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="S80" s="10" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="T80" s="10" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="75">
@@ -7218,23 +7215,23 @@
       </c>
       <c r="O81" s="9"/>
       <c r="P81" s="3" t="s">
-        <v>744</v>
+        <v>505</v>
       </c>
       <c r="Q81" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R81" s="10" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="S81" s="10" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="T81" s="10" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>